<commit_message>
Updated descriptions in libraries,...
sync'd up file name change in README
</commit_message>
<xml_diff>
--- a/PartsDB.xlsx
+++ b/PartsDB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="StdBx Parts" sheetId="1" r:id="rId1"/>
@@ -973,19 +973,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1334,8 +1345,8 @@
   </sheetPr>
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45:B47"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F32" sqref="A1:F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1347,646 +1358,649 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="7">
         <v>3.1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="9">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="9">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="9">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="9">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="9">
         <v>1</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="9">
         <v>1</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="9">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="9">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="9">
         <v>1</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="7" t="s">
         <v>270</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="9">
         <v>1</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="9">
         <v>1</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="9">
         <v>1</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="9">
         <v>1</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="9">
         <v>1</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="9">
         <v>1</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="9">
         <v>1</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="9">
         <v>1</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="9">
         <v>1</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="9">
         <v>1</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="9">
         <v>1</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="9">
         <v>1</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="9">
         <v>1</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="9">
         <v>1</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="9">
         <v>1</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="9">
         <v>1</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="9">
         <v>1</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="9">
         <v>1</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="9">
         <v>1</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="9">
         <v>1</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="7" t="s">
         <v>270</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="9">
         <v>1</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="7" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:F32">
+    <sortCondition ref="A2:A32"/>
+  </sortState>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="51" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -1996,7 +2010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
@@ -2056,7 +2070,7 @@
       <c r="G2" t="s">
         <v>242</v>
       </c>
-      <c r="H2" s="6"/>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2077,7 +2091,7 @@
       <c r="G3" t="s">
         <v>243</v>
       </c>
-      <c r="H3" s="6"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -2538,7 +2552,7 @@
       <c r="G26" t="s">
         <v>244</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="H26" s="3" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2561,7 +2575,7 @@
       <c r="G27" t="s">
         <v>244</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="H27" s="3" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2584,7 +2598,7 @@
       <c r="G28" t="s">
         <v>245</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="H28" s="3" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2607,7 +2621,7 @@
       <c r="G29" t="s">
         <v>245</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="H29" s="3" t="s">
         <v>167</v>
       </c>
     </row>

</xml_diff>